<commit_message>
umc pub_search update, prerelease
</commit_message>
<xml_diff>
--- a/data/processed/validations/mtm_othernr_manually_validated – 20250724.xlsx
+++ b/data/processed/validations/mtm_othernr_manually_validated – 20250724.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="592">
   <si>
     <t xml:space="preserve">trns_in_cluster</t>
   </si>
@@ -1765,6 +1765,39 @@
   </si>
   <si>
     <t xml:space="preserve">NCT03677401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004200-65_2016-004201-13_NCT03131648_NCT03160885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004200-65_NCT03131648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCT03131648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004200-65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP0162-1325</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004200-65_NCT03160885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCT03160885</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP0162-1326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004201-13_NCT03131648</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004201-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-004201-13_NCT03160885</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1936,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1965,6 +1998,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2319,12 +2360,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC1048576"/>
+  <dimension ref="A1:AO1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="U12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
-      <selection pane="bottomLeft" activeCell="AA23" activeCellId="0" sqref="AA23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="U117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
+      <selection pane="bottomLeft" activeCell="U133" activeCellId="0" sqref="U133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4194,12 +4235,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB21" s="7" t="s">
+      <c r="AA21" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB21" s="7"/>
       <c r="AC21" s="7" t="s">
         <v>127</v>
       </c>
@@ -4287,12 +4326,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA22" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB22" s="7" t="s">
+      <c r="AA22" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB22" s="7"/>
       <c r="AC22" s="7" t="s">
         <v>127</v>
       </c>
@@ -4380,12 +4417,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB23" s="7" t="s">
+      <c r="AA23" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB23" s="7"/>
       <c r="AC23" s="7" t="s">
         <v>127</v>
       </c>
@@ -4473,12 +4508,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA24" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB24" s="7" t="s">
+      <c r="AA24" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB24" s="7"/>
       <c r="AC24" s="7" t="s">
         <v>127</v>
       </c>
@@ -4566,12 +4599,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA25" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB25" s="7" t="s">
+      <c r="AA25" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB25" s="7"/>
       <c r="AC25" s="7" t="s">
         <v>127</v>
       </c>
@@ -4659,12 +4690,10 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AA26" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB26" s="7" t="s">
+      <c r="AA26" s="7" t="s">
         <v>33</v>
       </c>
+      <c r="AB26" s="7"/>
       <c r="AC26" s="7" t="s">
         <v>127</v>
       </c>
@@ -13586,7 +13615,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="131" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="n">
         <v>4</v>
       </c>
@@ -13618,6 +13647,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="K131" s="1"/>
       <c r="L131" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -13658,11 +13688,25 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="X131" s="1"/>
+      <c r="Y131" s="1"/>
       <c r="AA131" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AD131" s="1"/>
+      <c r="AE131" s="1"/>
+      <c r="AF131" s="1"/>
+      <c r="AG131" s="1"/>
+      <c r="AH131" s="1"/>
+      <c r="AI131" s="1"/>
+      <c r="AJ131" s="1"/>
+      <c r="AK131" s="1"/>
+      <c r="AL131" s="1"/>
+      <c r="AM131" s="1"/>
+      <c r="AN131" s="1"/>
+      <c r="AO131" s="1"/>
     </row>
-    <row r="132" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="n">
         <v>4</v>
       </c>
@@ -13694,6 +13738,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="K132" s="1"/>
       <c r="L132" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -13734,11 +13779,25 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="X132" s="1"/>
+      <c r="Y132" s="1"/>
       <c r="AA132" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AD132" s="1"/>
+      <c r="AE132" s="1"/>
+      <c r="AF132" s="1"/>
+      <c r="AG132" s="1"/>
+      <c r="AH132" s="1"/>
+      <c r="AI132" s="1"/>
+      <c r="AJ132" s="1"/>
+      <c r="AK132" s="1"/>
+      <c r="AL132" s="1"/>
+      <c r="AM132" s="1"/>
+      <c r="AN132" s="1"/>
+      <c r="AO132" s="1"/>
     </row>
-    <row r="133" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="n">
         <v>4</v>
       </c>
@@ -13818,11 +13877,25 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="X133" s="1"/>
+      <c r="Y133" s="1"/>
       <c r="AA133" s="1" t="s">
         <v>572</v>
       </c>
+      <c r="AD133" s="1"/>
+      <c r="AE133" s="1"/>
+      <c r="AF133" s="1"/>
+      <c r="AG133" s="1"/>
+      <c r="AH133" s="1"/>
+      <c r="AI133" s="1"/>
+      <c r="AJ133" s="1"/>
+      <c r="AK133" s="1"/>
+      <c r="AL133" s="1"/>
+      <c r="AM133" s="1"/>
+      <c r="AN133" s="1"/>
+      <c r="AO133" s="1"/>
     </row>
-    <row r="134" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="n">
         <v>3</v>
       </c>
@@ -13854,6 +13927,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="K134" s="1"/>
       <c r="L134" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -13894,14 +13968,28 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="X134" s="1"/>
+      <c r="Y134" s="1"/>
       <c r="AA134" s="1" t="s">
         <v>33</v>
       </c>
       <c r="AC134" s="1" t="s">
         <v>541</v>
       </c>
+      <c r="AD134" s="1"/>
+      <c r="AE134" s="1"/>
+      <c r="AF134" s="1"/>
+      <c r="AG134" s="1"/>
+      <c r="AH134" s="1"/>
+      <c r="AI134" s="1"/>
+      <c r="AJ134" s="1"/>
+      <c r="AK134" s="1"/>
+      <c r="AL134" s="1"/>
+      <c r="AM134" s="1"/>
+      <c r="AN134" s="1"/>
+      <c r="AO134" s="1"/>
     </row>
-    <row r="135" s="1" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="n">
         <v>3</v>
       </c>
@@ -13981,15 +14069,395 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+      <c r="X135" s="1"/>
+      <c r="Y135" s="1"/>
       <c r="AA135" s="1" t="s">
         <v>579</v>
       </c>
       <c r="AC135" s="1" t="s">
         <v>541</v>
       </c>
+      <c r="AD135" s="1"/>
+      <c r="AE135" s="1"/>
+      <c r="AF135" s="1"/>
+      <c r="AG135" s="1"/>
+      <c r="AH135" s="1"/>
+      <c r="AI135" s="1"/>
+      <c r="AJ135" s="1"/>
+      <c r="AK135" s="1"/>
+      <c r="AL135" s="1"/>
+      <c r="AM135" s="1"/>
+      <c r="AN135" s="1"/>
+      <c r="AO135" s="1"/>
     </row>
-    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A136" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="F136" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G136" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H136" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I136" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J136" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K136" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L136" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="N136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P136" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q136" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R136" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S136" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T136" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U136" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="V136" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="W136" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X136" s="1"/>
+      <c r="Y136" s="1"/>
+      <c r="AA136" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="AB136" s="0"/>
+      <c r="AC136" s="0"/>
+    </row>
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="F137" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G137" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H137" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J137" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K137" s="1"/>
+      <c r="L137" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N137" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O137" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P137" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q137" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R137" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S137" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T137" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U137" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="V137" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="W137" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X137" s="1"/>
+      <c r="Y137" s="1"/>
+      <c r="AA137" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB137" s="0"/>
+      <c r="AC137" s="0"/>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="F138" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G138" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H138" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J138" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K138" s="1"/>
+      <c r="L138" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P138" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q138" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R138" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S138" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T138" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U138" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="V138" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="W138" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X138" s="1"/>
+      <c r="Y138" s="1"/>
+      <c r="AA138" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB138" s="0"/>
+      <c r="AC138" s="0"/>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="F139" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G139" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H139" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I139" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J139" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K139" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L139" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N139" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="P139" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q139" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R139" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S139" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="T139" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U139" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="V139" s="0" t="s">
+        <v>588</v>
+      </c>
+      <c r="W139" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="X139" s="1"/>
+      <c r="Y139" s="1"/>
+      <c r="AA139" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="AB139" s="0"/>
+      <c r="AC139" s="0"/>
+    </row>
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Q140" s="0"/>
+      <c r="R140" s="0"/>
+      <c r="S140" s="0"/>
+      <c r="T140" s="0"/>
+      <c r="U140" s="0"/>
+      <c r="V140" s="0"/>
+      <c r="Z140" s="0"/>
+      <c r="AA140" s="0"/>
+      <c r="AB140" s="0"/>
+      <c r="AC140" s="0"/>
+    </row>
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Q141" s="0"/>
+      <c r="R141" s="0"/>
+      <c r="S141" s="0"/>
+      <c r="T141" s="0"/>
+      <c r="U141" s="0"/>
+      <c r="V141" s="0"/>
+      <c r="Z141" s="0"/>
+      <c r="AA141" s="0"/>
+      <c r="AB141" s="0"/>
+      <c r="AC141" s="0"/>
+    </row>
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Q142" s="0"/>
+      <c r="R142" s="0"/>
+      <c r="S142" s="0"/>
+      <c r="T142" s="0"/>
+      <c r="U142" s="0"/>
+      <c r="V142" s="0"/>
+      <c r="Z142" s="0"/>
+      <c r="AA142" s="0"/>
+      <c r="AB142" s="0"/>
+      <c r="AC142" s="0"/>
+    </row>
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Q143" s="0"/>
+      <c r="R143" s="0"/>
+      <c r="S143" s="0"/>
+      <c r="T143" s="0"/>
+      <c r="U143" s="0"/>
+      <c r="V143" s="0"/>
+      <c r="Z143" s="0"/>
+      <c r="AA143" s="0"/>
+      <c r="AB143" s="0"/>
+      <c r="AC143" s="0"/>
+    </row>
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Q144" s="0"/>
+      <c r="R144" s="0"/>
+      <c r="S144" s="0"/>
+      <c r="T144" s="0"/>
+      <c r="U144" s="0"/>
+      <c r="V144" s="0"/>
+      <c r="Z144" s="0"/>
+      <c r="AA144" s="0"/>
+      <c r="AB144" s="0"/>
+      <c r="AC144" s="0"/>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>